<commit_message>
update timesheet by jason
</commit_message>
<xml_diff>
--- a/Agenda_Minutes_Timesheet/Time sheet/Timetsheet - Ng Yiu Yeung.xlsx
+++ b/Agenda_Minutes_Timesheet/Time sheet/Timetsheet - Ng Yiu Yeung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Desktop/MCI_2021/MCI_Project/Team-024/Agenda_Minutes_Timesheet/Time sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FCB977-731A-9F48-B4A8-9ED43FFE1E17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38FC220-EAEE-9D4B-8E76-A48C66FACBBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14540" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40" yWindow="500" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 2 " sheetId="3" r:id="rId1"/>
@@ -18,8 +18,13 @@
     <sheet name="Week 4" sheetId="6" r:id="rId3"/>
     <sheet name="Week 5" sheetId="7" r:id="rId4"/>
     <sheet name="Week 6" sheetId="8" r:id="rId5"/>
-    <sheet name="Week 7" sheetId="9" r:id="rId6"/>
-    <sheet name="Week 8" sheetId="10" r:id="rId7"/>
+    <sheet name="Mid-sem break week 1" sheetId="9" r:id="rId6"/>
+    <sheet name="Mid-sem break week 2" sheetId="10" r:id="rId7"/>
+    <sheet name="Week 7" sheetId="14" r:id="rId8"/>
+    <sheet name="Week 8" sheetId="15" r:id="rId9"/>
+    <sheet name="Week 9" sheetId="17" r:id="rId10"/>
+    <sheet name="Week 10" sheetId="19" r:id="rId11"/>
+    <sheet name="Week 11" sheetId="21" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Week 2 '!$A$1:$H$13</definedName>
@@ -47,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="112">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -291,6 +296,102 @@
   </si>
   <si>
     <t>Complete another 10 % of the ionic course section 6</t>
+  </si>
+  <si>
+    <t>Ready for milestone 1 presentation to client</t>
+  </si>
+  <si>
+    <t>Complete milestone 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milestone 2 plan </t>
+  </si>
+  <si>
+    <t>Complete milestone 1</t>
+  </si>
+  <si>
+    <t>Complete another 10 % of the ionic course section 7</t>
+  </si>
+  <si>
+    <t>Complete another 15 % of the ionic course section 7</t>
+  </si>
+  <si>
+    <t>Complete another 20 % of the ionic course section 7</t>
+  </si>
+  <si>
+    <t>Milestone 2 execution</t>
+  </si>
+  <si>
+    <t>Report progress of milestone 2</t>
+  </si>
+  <si>
+    <t>Continue completing milestone 2</t>
+  </si>
+  <si>
+    <t>Complete another 40 % of the ionic course section 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working on HTTP request to create reflection and store in database </t>
+  </si>
+  <si>
+    <t>Main function of "Insight" page</t>
+  </si>
+  <si>
+    <t>Http request for "Timeline" page</t>
+  </si>
+  <si>
+    <t>Continue to finish this http request</t>
+  </si>
+  <si>
+    <t>Testing plan</t>
+  </si>
+  <si>
+    <t>Working on HTTP request to  retrieve data from database and show it in "Timeline" page</t>
+  </si>
+  <si>
+    <t>Main function of "Timeline" page</t>
+  </si>
+  <si>
+    <t>Testing plan for implementing testing</t>
+  </si>
+  <si>
+    <t>Writing testing code</t>
+  </si>
+  <si>
+    <t>Testing code</t>
+  </si>
+  <si>
+    <t>Automatic testing</t>
+  </si>
+  <si>
+    <t>Update testing plan</t>
+  </si>
+  <si>
+    <t>Internal group meeting for poster issue</t>
+  </si>
+  <si>
+    <t>Poster as a summary of project</t>
+  </si>
+  <si>
+    <t>Poster submission</t>
+  </si>
+  <si>
+    <t>Poster</t>
+  </si>
+  <si>
+    <t>Poster review on the coming Sat</t>
+  </si>
+  <si>
+    <t>Code review</t>
+  </si>
+  <si>
+    <t>Code style and organization of the code</t>
+  </si>
+  <si>
+    <t>Preparation work for final demo</t>
+  </si>
+  <si>
+    <t>Demo presentation</t>
   </si>
 </sst>
 </file>
@@ -1397,6 +1498,704 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5C769E-887C-E449-9359-E94C29568739}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="35.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D5" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="17">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.625</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="17">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="12">
+        <v>7</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="23">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="E8" s="12">
+        <v>5</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="23">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E9" s="12">
+        <v>6</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="E10" s="12">
+        <v>3</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8">
+        <f>SUM(E5:E10)</f>
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C5:D10" xr:uid="{A166FAED-1ECD-EA4E-B438-AAD97373EC7F}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D0C30A-14AB-9C4F-9B2C-C55D45EFCF76}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D5" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="12">
+        <v>3</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="17">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.625</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
+    </row>
+    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="17">
+        <v>0.375</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E7" s="12">
+        <v>7</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="23">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="E8" s="12">
+        <v>8</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="23">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="E9" s="12">
+        <v>4</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8">
+        <f>SUM(E5:E10)</f>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C5:D10" xr:uid="{74BE1C0F-4DBA-7C48-B864-A02096A89560}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C09D32-7617-0244-BCB3-9A075460CE35}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D5" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="17">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.625</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="17">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="12">
+        <v>7</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="23">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="E8" s="12">
+        <v>5</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="23">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E9" s="12">
+        <v>6</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="21">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8">
+        <f>SUM(E5:E10)</f>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C5:D10" xr:uid="{1A58267C-DF13-F14F-B767-042AC4CFE1EC}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
@@ -2880,7 +3679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E57F0CE-B4FB-2848-8FF7-4DF110FCC13C}">
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -3312,8 +4111,476 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A492DFD-6522-0A44-A5A1-C7AD6BB3DFF5}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D5" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="17">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E7" s="12">
+        <v>5</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="23">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="E8" s="12">
+        <v>5</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="23">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E9" s="12">
+        <v>6</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8">
+        <f>SUM(E5:E10)</f>
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C5:D10" xr:uid="{0A1EEDF4-5127-8B4D-8BFD-2622E0EEF492}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B8763C-31E9-2B4B-8FF0-2A21314DAC07}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D5" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E5" s="12">
+        <v>1</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="17">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D6" s="17">
+        <v>0.625</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="17">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E7" s="12">
+        <v>6</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="23">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="E8" s="12">
+        <v>5</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="23">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="12">
+        <v>7</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E10" s="12">
+        <v>3</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8">
+        <f>SUM(E5:E10)</f>
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C5:D10" xr:uid="{AC73411C-FC40-2245-AB44-7F5027D4C260}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555556</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7CE5D7E-071F-0C4C-B57C-48C1C6DE3779}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3355,7 +4622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -3387,10 +4654,10 @@
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="21">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="D5" s="21">
-        <v>0.41666666666666669</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E5" s="12">
         <v>1</v>
@@ -3423,10 +4690,10 @@
         <v>39</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -3450,7 +4717,7 @@
         <v>25</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -3474,7 +4741,7 @@
         <v>25</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -3498,7 +4765,7 @@
         <v>25</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3507,22 +4774,22 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="21">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="D10" s="21">
         <v>0.70833333333333337</v>
       </c>
       <c r="E10" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>73</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -3531,7 +4798,7 @@
       </c>
       <c r="E11" s="8">
         <f>SUM(E5:E10)</f>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3539,7 +4806,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C5:D10" xr:uid="{0A1EEDF4-5127-8B4D-8BFD-2622E0EEF492}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." sqref="C5:D10" xr:uid="{8FE6FDB3-0D9B-C947-AC40-F725F963C94A}">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>

</xml_diff>